<commit_message>
Serving CSS using FLASK rendered link rather than CSS file
</commit_message>
<xml_diff>
--- a/flask_web_project_for_data_representation/analysis.xlsx
+++ b/flask_web_project_for_data_representation/analysis.xlsx
@@ -436,240 +436,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>India farmers: Misleading content shared about the protests</t>
+          <t>No Flight Can Truly Be COVID-Free</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-asia-india-55157714</t>
+          <t>https://lifehacker.com/no-flight-can-truly-be-covid-free-1845898434</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>New York-based indoor ag company Gotham Greens raises $87 million</t>
+          <t>We Have Two COVID Vaccines Now</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://techcrunch.com/2020/12/08/new-york-based-indoor-ag-company-gotham-greens-raises-87-million/</t>
+          <t>https://vitals.lifehacker.com/we-have-two-covid-vaccines-now-1845913299</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Yeah, NASA can grow radishes in space now — Future Blink</t>
+          <t>What’s Up With the Latest COVID Relief Bill?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://mashable.com/video/nasa-grows-radish-in-space/</t>
+          <t>https://twocents.lifehacker.com/what-s-up-with-the-latest-covid-relief-bill-1845827491</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Why Alibaba rival Pinduoduo is investing in agritech</t>
+          <t>What We Know About Allergic Reactions to the COVID Vaccines</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://techcrunch.com/2020/12/16/pinduoduo-agritech/</t>
+          <t>https://vitals.lifehacker.com/what-we-know-about-allergic-reactions-to-the-covid-vacc-1845934680</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Norways Mowi loses fish farming permits in parts of Canada from 2022 - Reuters India</t>
+          <t>What to Do If Youre Exposed to COVID-19</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/mowi-canada-idINL1N2IY0E9</t>
+          <t>https://lifehacker.com/what-to-do-if-youre-exposed-to-covid-19-1845860079</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Singapore is the first country to approve the sale of lab-grown meat</t>
+          <t>What Will It Feel Like to Get a COVID Vaccine?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.engadget.com/singapore-eat-just-chicken-230119555.html</t>
+          <t>https://vitals.lifehacker.com/what-will-it-feel-like-to-get-a-covid-vaccine-1845810703</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Thousands protest in London against Indias farming reforms - Reuters</t>
+          <t>Were Probably Days Away From a COVID Vaccine</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/us-india-farms-protests-britain-idUSKBN28G0O0</t>
+          <t>https://vitals.lifehacker.com/were-probably-days-away-from-a-covid-vaccine-1845861896</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Thousands protest in London against Indias farming reforms - Reuters Canada</t>
+          <t>Dont Spit on the Ground During a Pandemic (Or Ever)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://ca.reuters.com/article/us-india-farms-protests-britain-idCAKBN28G0O0</t>
+          <t>https://lifehacker.com/dont-spit-on-the-ground-during-a-pandemic-or-ever-1845914513</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Biden Picks Marcia Fudge for HUD and Tom Vilsack for Agriculture Secretary</t>
+          <t>Californias COVID-19 exposure notification app starts rolling out</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2020/12/08/us/politics/marcia-fudge-hud-tom-vilsack-agriculture.html</t>
+          <t>https://www.engadget.com/california-covid-19-exposure-notification-app-235001952.html</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UK minister says Brexit trade talks are in the final few days - Reuters</t>
+          <t>The Free Market Approach to This Pandemic Isnt Working</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/britain-eu-talks-timescale-idUSS8N2DU0AI</t>
+          <t>https://www.wired.com/story/the-free-market-approach-to-this-pandemic-isnt-working/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UPDATE 1-Thousands protest in London against Indias farming reforms - Reuters India</t>
+          <t>Facebook adds new notifications for COVID-19 misinformation</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/india-farms-protests-britain-idINKBN28G0NV</t>
+          <t>https://www.engadget.com/facebook-notifications-harmful-coronavirus-misinformation-191233820.html</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Yara plans CO2-free ammonia plant in farming and shipping shift - Reuters India</t>
+          <t>Congress approves COVID-19 spending bill with contentious copyright measures</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/yara-esg-idINKBN28H1FM</t>
+          <t>https://www.engadget.com/covid-19-spending-bill-passes-with-new-streaming-copyright-law-tacked-on-102046838.html</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Yara plans CO2-free ammonia plant in farming and shipping shift - Reuters</t>
+          <t>Twitter will start removing COVID-19 vaccine misinformation next week</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/yara-esg-idUSKBN28H1FM</t>
+          <t>https://www.engadget.com/twitter-covid-19-vaccine-misinformation-policy-204452958.html</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UK farming minister says EU talks will continue until no point doing so - Reuters</t>
+          <t>Covid-19: How Covid cruise ships are navigating troubled waters</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/us-britain-eu-talks-eustice-idUSKBN28G07S</t>
+          <t>https://www.bbc.co.uk/news/av/world-55241333</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Missing: 50,000 Salmon</t>
+          <t>The Last, ‘Ultra-Cold’ Mile for Covid-19 Vaccines</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://earther.gizmodo.com/missing-50-000-salmon-1845750619</t>
+          <t>https://www.wired.com/story/the-last-ultra-cold-mile-for-covid-19-vaccines/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Environment to benefit from ‘biggest farming shake-up in 50 years’</t>
+          <t>Conferences After Covid Will Be Shorter—and Smarter</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://amp.theguardian.comenvironment/2020/nov/30/environment-to-benefit-from-biggest-farming-shake-up-in-50-years</t>
+          <t>https://www.wired.com/story/what-conferences-will-look-like-post-covid/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Debra White Plume, Defender of Her Tribe, Is Dead at 66</t>
+          <t>The ‘Healthy Building’ Surge Will Outlast the Pandemic</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2020/11/27/us/debra-white-dead.html</t>
+          <t>https://www.wired.com/story/healthy-building-outlast-pandemic/</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Japfa in $236 mln deal with buyout funds for Indonesian dairy business - Reuters India</t>
+          <t>A Clever Strategy to Distribute Covid Aid—With Satellite Data</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/japfa-ma-investment-idINL4N2IN0RA</t>
+          <t>https://www.wired.com/story/clever-strategy-distribute-covid-aid-satellite-data/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Vegetable-growing reaches new heights in Copenhagen - Reuters India</t>
+          <t>Poland’s GeneMe secures €5.2M seed funding for its rapid COVID-19 test</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/denmark-vertical-farming-idINKBN28J1V2</t>
+          <t>http://techcrunch.com/2020/12/17/polands-geneme-secures-e5-2m-seed-funding-for-its-rapid-covid-19-test/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Vegetable-growing reaches new heights in Copenhagen - Reuters</t>
+          <t>Twitter says it will start removing COVID-19 vaccine misinformation</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/denmark-vertical-farming-idUSKBN28J1V2</t>
+          <t>https://www.theverge.com/2020/12/16/22179074/twitter-coronavirus-misinformation-covid19-vaccine-vaccination-label</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
making backup of work while trying to fix matplot lib saving
</commit_message>
<xml_diff>
--- a/flask_web_project_for_data_representation/analysis.xlsx
+++ b/flask_web_project_for_data_representation/analysis.xlsx
@@ -436,240 +436,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>No Flight Can Truly Be COVID-Free</t>
+          <t>Ebola Species Thought to Be Harmless to Humans Can Sicken Pigs, Raising Alarm Bells</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://lifehacker.com/no-flight-can-truly-be-covid-free-1845898434</t>
+          <t>https://gizmodo.com/ebola-species-thought-to-be-harmless-to-humans-can-sick-1845934257</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>We Have Two COVID Vaccines Now</t>
+          <t>Czech golden pig ornaments get mask for COVID Christmas - Reuters India</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://vitals.lifehacker.com/we-have-two-covid-vaccines-now-1845913299</t>
+          <t>https://in.reuters.com/article/christmas-season-czech-decoration-pigs-idINKBN28C1VX</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>What’s Up With the Latest COVID Relief Bill?</t>
+          <t>Czech golden pig ornaments get mask for COVID Christmas - Reuters</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://twocents.lifehacker.com/what-s-up-with-the-latest-covid-relief-bill-1845827491</t>
+          <t>https://www.reuters.com/article/us-christmas-season-czech-decoration-pig-idUSKBN28C1SY</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>What We Know About Allergic Reactions to the COVID Vaccines</t>
+          <t>Are we guinea pigs? - Frances seniors wary of COVID vaccine - Reuters India</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://vitals.lifehacker.com/what-we-know-about-allergic-reactions-to-the-covid-vacc-1845934680</t>
+          <t>https://in.reuters.com/article/health-coronavirus-france-seniors-idINL8N2IV2O5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>What to Do If Youre Exposed to COVID-19</t>
+          <t>Amid pandemic, orders soar for Brazil robot that feeds pigs playing classical music - Reuters India</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://lifehacker.com/what-to-do-if-youre-exposed-to-covid-19-1845860079</t>
+          <t>https://in.reuters.com/article/brazil-pig-farming-technology-idINKBN28E0BU</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>What Will It Feel Like to Get a COVID Vaccine?</t>
+          <t>Amid pandemic, orders soar for Brazil robot that feeds pigs playing classical music - Reuters UK</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://vitals.lifehacker.com/what-will-it-feel-like-to-get-a-covid-vaccine-1845810703</t>
+          <t>https://uk.reuters.com/article/us-brazil-pig-farming-technology-idUKKBN28D3F3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Were Probably Days Away From a COVID Vaccine</t>
+          <t>Are we guinea pigs? - Frances seniors wary of COVID vaccine - Reuters India</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://vitals.lifehacker.com/were-probably-days-away-from-a-covid-vaccine-1845861896</t>
+          <t>https://www.reuters.com/article/health-coronavirus-france-seniors-idINKBN28P2ET</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dont Spit on the Ground During a Pandemic (Or Ever)</t>
+          <t>Googles AR animal farm now includes pigs, milk cows, and more</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://lifehacker.com/dont-spit-on-the-ground-during-a-pandemic-or-ever-1845914513</t>
+          <t>https://www.androidcentral.com/google-adds-50-new-3d-animals-its-ar-collection</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Californias COVID-19 exposure notification app starts rolling out</t>
+          <t>How Much Watching Time Do You Have This Weekend?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.engadget.com/california-covid-19-exposure-notification-app-235001952.html</t>
+          <t>https://www.nytimes.com/2020/12/10/arts/television/pennyworth-wilds-couples-therapy.html</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>The Free Market Approach to This Pandemic Isnt Working</t>
+          <t>California Governor Blocks Release of Manson Follower Leslie Van Houten</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.wired.com/story/the-free-market-approach-to-this-pandemic-isnt-working/</t>
+          <t>https://www.nytimes.com/2020/11/29/us/Charles-manson-Leslie-van-Houten.html</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Facebook adds new notifications for COVID-19 misinformation</t>
+          <t>Germany continues talks with China over pork import bans - Reuters UK</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.engadget.com/facebook-notifications-harmful-coronavirus-misinformation-191233820.html</t>
+          <t>https://uk.reuters.com/article/germany-swinefever-china-idUKL8N2IQ1O4</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Congress approves COVID-19 spending bill with contentious copyright measures</t>
+          <t>Germany continues talks with China over pork import bans - Reuters India</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.engadget.com/covid-19-spending-bill-passes-with-new-streaming-copyright-law-tacked-on-102046838.html</t>
+          <t>https://in.reuters.com/article/germany-swinefever-china-idINL8N2IQ1O4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Twitter will start removing COVID-19 vaccine misinformation next week</t>
+          <t>Can You Bring Your Emotional Support Animal on Your Next Flight?</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.engadget.com/twitter-covid-19-vaccine-misinformation-policy-204452958.html</t>
+          <t>https://twocents.lifehacker.com/can-you-bring-your-emotional-support-animal-on-your-nex-1845800941</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Covid-19: How Covid cruise ships are navigating troubled waters</t>
+          <t>"Deck the Halls with War Pigs," a Black Sabbath yuletide mash-up for the ages</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/av/world-55241333</t>
+          <t>https://boingboing.net/2020/12/17/deck-the-halls-with-war-pigs-a-black-sabbath-yuletide-mash-up-for-the-ages.html</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The Last, ‘Ultra-Cold’ Mile for Covid-19 Vaccines</t>
+          <t>Googles library of AR animals grows, welcoming zebras, giraffes, chow chows, and more</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.wired.com/story/the-last-ultra-cold-mile-for-covid-19-vaccines/</t>
+          <t>https://mashable.com/article/google-ar-animals-zebra-giraffe-50-new/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Conferences After Covid Will Be Shorter—and Smarter</t>
+          <t>Flush with cash, Chinese hog producer builds worlds largest pig farm - Reuters UK</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.wired.com/story/what-conferences-will-look-like-post-covid/</t>
+          <t>https://uk.reuters.com/article/uk-china-swinefever-muyuanfoods-idUKKBN28H0C8</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>The ‘Healthy Building’ Surge Will Outlast the Pandemic</t>
+          <t>Flush with cash, Chinese hog producer builds worlds largest pig farm - Reuters</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.wired.com/story/healthy-building-outlast-pandemic/</t>
+          <t>https://www.reuters.com/article/us-china-swinefever-muyuanfoods-idUSKBN28H0CC</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>A Clever Strategy to Distribute Covid Aid—With Satellite Data</t>
+          <t>German minister urges meatpackers to work overtime to clear farm backlog - Reuters.com</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.wired.com/story/clever-strategy-distribute-covid-aid-satellite-data/</t>
+          <t>https://www.reuters.com/article/us-germany-meat-market-idINKBN28713J</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Poland’s GeneMe secures €5.2M seed funding for its rapid COVID-19 test</t>
+          <t>German minister urges meatpackers to work overtime to clear farm backlog - Reuters UK</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>http://techcrunch.com/2020/12/17/polands-geneme-secures-e5-2m-seed-funding-for-its-rapid-covid-19-test/</t>
+          <t>https://uk.reuters.com/article/us-germany-meat-market-idUKKBN28713J</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Twitter says it will start removing COVID-19 vaccine misinformation</t>
+          <t>Tyson Foods idles production at Iowa pork plant after system malfunction - Reuters UK</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.theverge.com/2020/12/16/22179074/twitter-coronavirus-misinformation-covid19-vaccine-vaccination-label</t>
+          <t>https://uk.reuters.com/article/tyson-plant-iowa-idUKL4N2IW3YO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
working with the concept flask send file to return image
</commit_message>
<xml_diff>
--- a/flask_web_project_for_data_representation/analysis.xlsx
+++ b/flask_web_project_for_data_representation/analysis.xlsx
@@ -436,240 +436,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ebola Species Thought to Be Harmless to Humans Can Sicken Pigs, Raising Alarm Bells</t>
+          <t>A ‘Messiah’ for the Multitudes, Freed From History’s Bonds</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://gizmodo.com/ebola-species-thought-to-be-harmless-to-humans-can-sick-1845934257</t>
+          <t>https://www.nytimes.com/2020/12/21/arts/music/handel-messiah-canada-indigenous.html</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Czech golden pig ornaments get mask for COVID Christmas - Reuters India</t>
+          <t>Sonos launches microphone-free Arc SL soundbar exclusively at Costco</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/christmas-season-czech-decoration-pigs-idINKBN28C1VX</t>
+          <t>https://www.theverge.com/2020/12/2/22011112/sonos-arc-sl-no-microphone-now-available-costco</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Czech golden pig ornaments get mask for COVID Christmas - Reuters</t>
+          <t>Canada bans mass exports of prescription drugs</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/us-christmas-season-czech-decoration-pig-idUSKBN28C1SY</t>
+          <t>https://www.bbc.co.uk/news/world-us-canada-55119428</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Are we guinea pigs? - Frances seniors wary of COVID vaccine - Reuters India</t>
+          <t>Canada Sixties Scoop: Indigenous survivors map out their stories</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/health-coronavirus-france-seniors-idINL8N2IV2O5</t>
+          <t>https://www.bbc.co.uk/news/av/world-us-canada-55269251</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Amid pandemic, orders soar for Brazil robot that feeds pigs playing classical music - Reuters India</t>
+          <t>Gatik’s self-driving box trucks to shuttle groceries for Loblaw in Canada</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/brazil-pig-farming-technology-idINKBN28E0BU</t>
+          <t>http://techcrunch.com/2020/11/23/gatiks-self-driving-box-trucks-to-shuttle-groceries-for-loblaw-in-canada/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Amid pandemic, orders soar for Brazil robot that feeds pigs playing classical music - Reuters UK</t>
+          <t>BRIEF-Canada PM Trudeau says first batch Of Pfizer/BioNTech vaccines arrived in Canada - Reuters India</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/us-brazil-pig-farming-technology-idUKKBN28D3F3</t>
+          <t>https://in.reuters.com/article/brief-canada-pm-trudeau-says-first-batch-idINL1N2IU01V</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Are we guinea pigs? - Frances seniors wary of COVID vaccine - Reuters India</t>
+          <t>BRIEF-Canada PM Trudeau says first batch Of Pfizer/BioNTech vaccines arrived in Canada - Reuters India</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/health-coronavirus-france-seniors-idINKBN28P2ET</t>
+          <t>https://in.reuters.com/article/brief-canada-pm-trudeau-says-first-batch-idUKL1N2IU01V</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Googles AR animal farm now includes pigs, milk cows, and more</t>
+          <t>Google’s Nest Hub Max smart screen can now make Zoom calls</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.androidcentral.com/google-adds-50-new-3d-animals-its-ar-collection</t>
+          <t>http://techcrunch.com/2020/12/14/googles-nest-hub-max-smart-screen-can-now-make-zoom-calls/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>How Much Watching Time Do You Have This Weekend?</t>
+          <t>Lightspeed acquires restaurant software company Upserve for $430M</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2020/12/10/arts/television/pennyworth-wilds-couples-therapy.html</t>
+          <t>http://techcrunch.com/2020/12/01/lightspeed-acquires-upserve/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>California Governor Blocks Release of Manson Follower Leslie Van Houten</t>
+          <t>ServiceNow is acquiring Element AI, the Canadian startup building AI services for enterprises</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2020/11/29/us/Charles-manson-Leslie-van-Houten.html</t>
+          <t>http://techcrunch.com/2020/11/30/servicenow-is-acquiring-element-ai-the-canadian-startup-building-ai-services-for-enterprises/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Germany continues talks with China over pork import bans - Reuters UK</t>
+          <t>Canada Is Latest to Approve Covid-19 Vaccine—and U.S. Is Likely Next</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/germany-swinefever-china-idUKL8N2IQ1O4</t>
+          <t>https://gizmodo.com/canada-is-latest-to-approve-covid-19-vaccine-and-u-s-i-1845844914</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Germany continues talks with China over pork import bans - Reuters India</t>
+          <t>Canada extends travel restrictions for those entering the country - Reuters Canada</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/germany-swinefever-china-idINL8N2IQ1O4</t>
+          <t>https://ca.reuters.com/article/us-health-coronavirus-canada-travel-idCAKBN2890XG</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Can You Bring Your Emotional Support Animal on Your Next Flight?</t>
+          <t>Amid surging second coronavirus wave, Canada to unveil more spending - Reuters Canada</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://twocents.lifehacker.com/can-you-bring-your-emotional-support-animal-on-your-nex-1845800941</t>
+          <t>https://ca.reuters.com/article/canada-budget-idCAKBN28A1AH</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>"Deck the Halls with War Pigs," a Black Sabbath yuletide mash-up for the ages</t>
+          <t>Defense grilling of Canada police witness in Huawei CFOs U.S. extradition case continues - Reuters Canada</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://boingboing.net/2020/12/17/deck-the-halls-with-war-pigs-a-black-sabbath-yuletide-mash-up-for-the-ages.html</t>
+          <t>https://ca.reuters.com/article/us-usa-huawei-tech-canada-idCAKBN2841E8</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Googles library of AR animals grows, welcoming zebras, giraffes, chow chows, and more</t>
+          <t>Canada plans digital tax in 2022 on global tech giants - Reuters Canada</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://mashable.com/article/google-ar-animals-zebra-giraffe-50-new/</t>
+          <t>https://ca.reuters.com/article/us-canada-budget-tax-idCAKBN28A2ZM</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Flush with cash, Chinese hog producer builds worlds largest pig farm - Reuters UK</t>
+          <t>Bank of Canada reiterates it could cut rates further if COVID worsens - Reuters Canada</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/uk-china-swinefever-muyuanfoods-idUKKBN28H0C8</t>
+          <t>https://ca.reuters.com/article/us-canada-cenbank-idCAKBN28K2WW</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Flush with cash, Chinese hog producer builds worlds largest pig farm - Reuters</t>
+          <t>Canada trade deficit shrinks slightly in October, still higher than expected - Reuters Canada</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/us-china-swinefever-muyuanfoods-idUSKBN28H0CC</t>
+          <t>https://ca.reuters.com/article/us-canada-economy-trade-idCAKBN28E2ZA</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>German minister urges meatpackers to work overtime to clear farm backlog - Reuters.com</t>
+          <t>CANADA FX DEBT-C$ climbs as market shrugs off Bank of Canada jawboning - Reuters India</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/us-germany-meat-market-idINKBN28713J</t>
+          <t>https://uk.reuters.com/article/canada-forex-idINL1N2IV2FS</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>German minister urges meatpackers to work overtime to clear farm backlog - Reuters UK</t>
+          <t>Air Canada makes more cuts in Atlantic Canada - CBC News</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/us-germany-meat-market-idUKKBN28713J</t>
+          <t>https://www.youtube.com/watch?v=m9AwKeuVfeU</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Tyson Foods idles production at Iowa pork plant after system malfunction - Reuters UK</t>
+          <t>Canadian Fashion Mogul Peter Nygard Indicted on Sex-Trafficking Charges</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/tyson-plant-iowa-idUKL4N2IW3YO</t>
+          <t>https://www.nytimes.com/2020/12/15/world/canada/peter-nygard-sex-trafficking-charges.html</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed issue of reporting matplotlib graph to web page
</commit_message>
<xml_diff>
--- a/flask_web_project_for_data_representation/analysis.xlsx
+++ b/flask_web_project_for_data_representation/analysis.xlsx
@@ -436,240 +436,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>India farmers: Misleading content shared about the protests</t>
+          <t>Stimulus, Brexit, Storm:Your Thursday Evening Briefing</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-asia-india-55157714</t>
+          <t>https://www.nytimes.com/2020/12/24/briefing/stimulus-brexit-storm.html</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>New York-based indoor ag company Gotham Greens raises $87 million</t>
+          <t>UKs Gove says: theres a chance of a no-deal Brexit - Reuters India</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://techcrunch.com/2020/12/08/new-york-based-indoor-ag-company-gotham-greens-raises-87-million/</t>
+          <t>https://www.reuters.com/article/uk-britain-eu-gove-idINKBN28B487</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Yeah, NASA can grow radishes in space now — Future Blink</t>
+          <t>UKs Gove says: theres a chance of a no-deal Brexit - Reuters UK</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://mashable.com/video/nasa-grows-radish-in-space/</t>
+          <t>https://uk.reuters.com/article/uk-britain-eu-gove-idUKKBN28B487</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Why Alibaba rival Pinduoduo is investing in agritech</t>
+          <t>EU sets out plans in case Brexit trade talks fail</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://techcrunch.com/2020/12/16/pinduoduo-agritech/</t>
+          <t>https://www.bbc.co.uk/news/world-europe-55259144</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Norways Mowi loses fish farming permits in parts of Canada from 2022 - Reuters India</t>
+          <t>UKs Gove sees scope for compromise on fish in Brexit talks - Reuters</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/mowi-canada-idINL1N2IY0E9</t>
+          <t>https://www.reuters.com/article/us-britain-eu-fish-idUSKBN28J0WU</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Singapore is the first country to approve the sale of lab-grown meat</t>
+          <t>UKs Gove sees scope for compromise on fish in Brexit talks - Reuters</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.engadget.com/singapore-eat-just-chicken-230119555.html</t>
+          <t>https://www.reuters.com/article/uk-britain-eu-fish-idUSKBN28J0X0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Thousands protest in London against Indias farming reforms - Reuters</t>
+          <t>Sterling holds above $1.33 on Brexit trade deal hopes - Reuters UK</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/us-india-farms-protests-britain-idUSKBN28G0O0</t>
+          <t>https://uk.reuters.com/article/uk-britain-sterling-idUKKBN28A10E</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Thousands protest in London against Indias farming reforms - Reuters Canada</t>
+          <t>Stena Line says role in UK delivery of Pfizer vaccine going well - Reuters UK</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://ca.reuters.com/article/us-india-farms-protests-britain-idCAKBN28G0O0</t>
+          <t>https://uk.reuters.com/article/uk-health-coronavirus-britain-stena-idUKKBN28E191</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Biden Picks Marcia Fudge for HUD and Tom Vilsack for Agriculture Secretary</t>
+          <t>UK cabinet to back Johnson over no-deal Brexit - The Times - Reuters</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2020/12/08/us/politics/marcia-fudge-hud-tom-vilsack-agriculture.html</t>
+          <t>https://www.reuters.com/article/uk-britain-eu-trade-idUSKBN28G010</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UK minister says Brexit trade talks are in the final few days - Reuters</t>
+          <t>FACTBOX-Higher prices, traffic jams: likely impact of Brexit impasse on businesses - Reuters</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/britain-eu-talks-timescale-idUSS8N2DU0AI</t>
+          <t>https://www.reuters.com/article/britain-eu-companies-idUSL8N2IN27C</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UPDATE 1-Thousands protest in London against Indias farming reforms - Reuters India</t>
+          <t>Sterling stabilises after Brexit deal hopes rebound - Reuters</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/india-farms-protests-britain-idINKBN28G0NV</t>
+          <t>https://www.reuters.com/article/britain-sterling-idUSKBN28P0XT</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Yara plans CO2-free ammonia plant in farming and shipping shift - Reuters India</t>
+          <t>EUs Barnier says "crucial" moment in UK trade talks - Reuters</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/yara-esg-idINKBN28H1FM</t>
+          <t>https://www.reuters.com/article/britain-eu-barnier-idUSKBN28U0J8</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Yara plans CO2-free ammonia plant in farming and shipping shift - Reuters</t>
+          <t>Factbox-Higher prices, traffic jams: likely impact of Brexit impasse on businesses - Reuters UK</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/yara-esg-idUSKBN28H1FM</t>
+          <t>https://uk.reuters.com/article/uk-britain-eu-companies-idUKKBN28K1P2</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UK farming minister says EU talks will continue until no point doing so - Reuters</t>
+          <t>EUs Barnier tells member states latest UK fish offer unacceptable - Reuters Canada</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/us-britain-eu-talks-eustice-idUSKBN28G07S</t>
+          <t>https://www.reuters.com/article/us-britain-eu-barnier-fish-idUSKBN28W214</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Missing: 50,000 Salmon</t>
+          <t>Rifts over fishing rights still blocking EU-UK trade deal - Reuters India</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://earther.gizmodo.com/missing-50-000-salmon-1845750619</t>
+          <t>https://in.reuters.com/article/us-britain-eu-idINKBN28W13M</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Environment to benefit from ‘biggest farming shake-up in 50 years’</t>
+          <t>Rifts over fishing rights still blocking EU-UK trade deal - Reuters</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://amp.theguardian.comenvironment/2020/nov/30/environment-to-benefit-from-biggest-farming-shake-up-in-50-years</t>
+          <t>https://www.reuters.com/article/uk-britain-eu-barnier-idUSKBN28W13U</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Debra White Plume, Defender of Her Tribe, Is Dead at 66</t>
+          <t>PRECIOUS-Gold gains on subdued dollar after Brexit trade deal - Reuters UK</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2020/11/27/us/debra-white-dead.html</t>
+          <t>https://in.reuters.com/article/global-precious-idUKL4N2J4274</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Japfa in $236 mln deal with buyout funds for Indonesian dairy business - Reuters India</t>
+          <t>Smoother glide path to Brexit trade deal after Northern Ireland accord, UKs Gove says - Reuters</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/japfa-ma-investment-idINL4N2IN0RA</t>
+          <t>https://www.reuters.com/article/britain-eu-gove-idUSKBN28J0PS</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Vegetable-growing reaches new heights in Copenhagen - Reuters India</t>
+          <t>PRECIOUS-Gold gains on subdued dollar after Brexit trade deal - Reuters UK</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/denmark-vertical-farming-idINKBN28J1V2</t>
+          <t>https://uk.reuters.com/article/global-precious-idUKL4N2J4274</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Vegetable-growing reaches new heights in Copenhagen - Reuters</t>
+          <t>Stena Line says role in UK delivery of Pfizer vaccine going well - Reuters</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/denmark-vertical-farming-idUSKBN28J1V2</t>
+          <t>https://www.reuters.com/article/uk-health-coronavirus-britain-stena-idUSKBN28E191</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated code to show location of spreadsheet with backslash formatting
</commit_message>
<xml_diff>
--- a/flask_web_project_for_data_representation/analysis.xlsx
+++ b/flask_web_project_for_data_representation/analysis.xlsx
@@ -436,240 +436,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Stimulus, Brexit, Storm:Your Thursday Evening Briefing</t>
+          <t>Pasteles Tere</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2020/12/24/briefing/stimulus-brexit-storm.html</t>
+          <t>https://fontsinuse.com/uses/37611/pasteles-tere?utm_source=feedburner&amp;utm_medium=feed&amp;utm_campaign=Feed%3A+FontsInUseAll+%28Fonts+In+Use%29</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>UKs Gove says: theres a chance of a no-deal Brexit - Reuters India</t>
+          <t>Bu Besinler Akciğerleri Güçlendiriyor!</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/uk-britain-eu-gove-idINKBN28B487</t>
+          <t>https://www.hurriyet.com.tr/mahmure/galeri-bu-besinler-akcigerleri-guclendiriyor-41695361</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>UKs Gove says: theres a chance of a no-deal Brexit - Reuters UK</t>
+          <t>Acusa panista de corrupción... a panista</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/uk-britain-eu-gove-idUKKBN28B487</t>
+          <t>https://www.reforma.com/libre/acceso/accesofb.htm?urlredirect=/acusa-panista-de-corrupcion-a-panista/ar2084120</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EU sets out plans in case Brexit trade talks fail</t>
+          <t>Qué es el último teorema de Fermat y por qué los matemáticos demoraron 3 siglos en resolverlo</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.bbc.co.uk/news/world-europe-55259144</t>
+          <t>https://www.bbc.com/mundo/noticias-55412805</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>UKs Gove sees scope for compromise on fish in Brexit talks - Reuters</t>
+          <t>¿Cómo sería México si Estados Unidos no se hubiera apropiado de más de la mitad de su territorio en el siglo XIX?</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/us-britain-eu-fish-idUSKBN28J0WU</t>
+          <t>https://www.bbc.com/mundo/noticias-55151922</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>UKs Gove sees scope for compromise on fish in Brexit talks - Reuters</t>
+          <t>Cómo se rige la Antártida, quién reclama su soberanía y por qué despierta tanto interés</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/uk-britain-eu-fish-idUSKBN28J0X0</t>
+          <t>https://www.bbc.com/mundo/noticias-internacional-55108222</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sterling holds above $1.33 on Brexit trade deal hopes - Reuters UK</t>
+          <t>Mantecadas al tren, las vendedoras que hicieron viajera la dulce tradición de Astorga (León)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/uk-britain-sterling-idUKKBN28A10E</t>
+          <t>https://www.eldiario.es/castilla-y-leon/provincias/leon/mantecadas-tren-vendedoras-hicieron-viajera-dulce-tradicion-astorga-leon_1_6623637.html</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Stena Line says role in UK delivery of Pfizer vaccine going well - Reuters UK</t>
+          <t>Tere otunun faydaları nelerdir? İç organları arındıran tere otu nasıl tüketilir?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/uk-health-coronavirus-britain-stena-idUKKBN28E191</t>
+          <t>https://www.haber7.com/saglik/haber/2992834-tere-otunun-faydalari-nelerdir-ic-organlari-arindiran-tere-otu-nasil-tuketilir</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>UK cabinet to back Johnson over no-deal Brexit - The Times - Reuters</t>
+          <t>Have bonded well with Akash Mukherjee: Aishwarya Raj Bhakuni</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/uk-britain-eu-trade-idUSKBN28G010</t>
+          <t>https://www.santabanta.com/bollywood/150620/have-bonded-well-with-akash-mukherjee-aishwarya-raj-bhakuni/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FACTBOX-Higher prices, traffic jams: likely impact of Brexit impasse on businesses - Reuters</t>
+          <t>Topul dezvoltatorilor de software din România, domeniu în care lucrează peste 130.000 de IT-işt</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/britain-eu-companies-idUSL8N2IN27C</t>
+          <t>https://economie.hotnews.ro/stiri-it-24454572-topul-dezvoltatorilor-software-din-romania-domeniu-care-lucreaza-peste-130-000-ist.htm</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sterling stabilises after Brexit deal hopes rebound - Reuters</t>
+          <t>Noi finanțări de 1-3 milioane Euro pentru startup-uri IT românști</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/britain-sterling-idUSKBN28P0XT</t>
+          <t>https://economie.hotnews.ro/stiri-eurofonduri-24454593-noi-finantari-1-3-milioane-euro-pentru-startup-uri-romansti.htm</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EUs Barnier says "crucial" moment in UK trade talks - Reuters</t>
+          <t>O familie din Iasi s-a mutat în Zanzibar din cauza restricţiilor Covid. "E mai ieftin aici de trăit"</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/britain-eu-barnier-idUSKBN28U0J8</t>
+          <t>https://www.hotnews.ro/stiri-coronavirus-24453771-familie-din-iasi-mutat-zanzibar-din-cauza-restrictiilor-covid-mai-ieftin-aici-trait.htm</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Factbox-Higher prices, traffic jams: likely impact of Brexit impasse on businesses - Reuters UK</t>
+          <t>​VIDEO Real Madrid, învinsă pentru a doua oară de Șahtior Donețk (2-0) / RB Salzburg, victorie în Rusia (3-1 vs Lokomotiv Moscova)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/uk-britain-eu-companies-idUKKBN28K1P2</t>
+          <t>https://sport.hotnews.ro/stiri-fotbal-24453467-video-sahtior-donetk-invinge-pentru-doua-oara-real-madrid-2-0-salzburg-victorie-rusia-3-1-lokomotiv-moscova.htm</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>EUs Barnier tells member states latest UK fish offer unacceptable - Reuters Canada</t>
+          <t>Mircea Rednic este noul antrenor al echipei FC Viitorul</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/us-britain-eu-barnier-fish-idUSKBN28W214</t>
+          <t>https://sport.hotnews.ro/stiri-fotbal-24453452-mircea-rednic-este-noul-antrenor-echipei-viitorul.htm</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Rifts over fishing rights still blocking EU-UK trade deal - Reuters India</t>
+          <t>Efectele pandemiei de COVID-19: Unul din 33 de locuitori ai lumii, număr record, va avea nevoie de ajutor pentru a supraviețui</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/us-britain-eu-idINKBN28W13M</t>
+          <t>https://www.hotnews.ro/stiri-international-24452405-efectele-pandemiei-covid-19-unul-din-33-locuitori-lumii-numar-record-avea-nevoie-ajutor-pentru-supravietui.htm</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Rifts over fishing rights still blocking EU-UK trade deal - Reuters</t>
+          <t>În Europa de Est publicul e menținut în afara consultărilor privind planul de redresare verde / În România, discuțiile s-au purtat în spatele ușilor închise (Emerging Europe)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/uk-britain-eu-barnier-idUSKBN28W13U</t>
+          <t>https://www.hotnews.ro/stiri-international-24453618-europa-est-publicul-mentinut-afara-consultarilor-privind-planul-redresare-verde-romania-discutiile-purtat-spatele-usilor-inchise-emerging-europe.htm</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PRECIOUS-Gold gains on subdued dollar after Brexit trade deal - Reuters UK</t>
+          <t>Reacție dură a Patriarhiei după ce CE a propus desfășurarea online a slujbelor: Nimeni onest sau ancorat în realitatea socială profundă nu poate dori sau impune acest lucru</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://in.reuters.com/article/global-precious-idUKL4N2J4274</t>
+          <t>https://www.hotnews.ro/stiri-esential-24454472-reactie-dura-patriarhiei-dupa-propus-desfasurarea-online-slujbelor-nimeni-onest-sau-ancorat-realitatea-sociala-profunda-nu-poate-dori-sau-impune-acest-lucru.htm</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Smoother glide path to Brexit trade deal after Northern Ireland accord, UKs Gove says - Reuters</t>
+          <t>Klaus Iohannis a decorat mai mulți doctori și asistente medicale, de Ziua Națională a României: Dvs, cei din linia întâi, luptați neobosit pentru viață, de multe ori cu riscul propriei siguranțe VIDEO</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/britain-eu-gove-idUSKBN28J0PS</t>
+          <t>https://www.hotnews.ro/stiri-esential-24453142-klaus-iohannis-decorat-mai-multi-doctori-asistente-medicale-ziua-nationala-romaniei-video.htm</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PRECIOUS-Gold gains on subdued dollar after Brexit trade deal - Reuters UK</t>
+          <t>Giuliani ar fi discutat cu Trump despre posibilă grațiere - presă</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://uk.reuters.com/article/global-precious-idUKL4N2J4274</t>
+          <t>https://www.hotnews.ro/stiri-international-24453261-giuliani-spus-discutat-posibila-gratiere-trump.htm</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Stena Line says role in UK delivery of Pfizer vaccine going well - Reuters</t>
+          <t>LISTĂ: Antreprenori IT români care s-au remarcat în anul 2020</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.reuters.com/article/uk-health-coronavirus-britain-stena-idUSKBN28E191</t>
+          <t>https://economie.hotnews.ro/stiri-it-24453329-lista-antreprenori-romani-care-remarcat-anul-2020.htm</t>
         </is>
       </c>
     </row>

</xml_diff>